<commit_message>
fixed tiebreak three teams
</commit_message>
<xml_diff>
--- a/xlsx/tied_three_eu.xlsx
+++ b/xlsx/tied_three_eu.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aldi\Documents\GitHub\tiebreak_wc\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ALESSANDRO\Documents\GitHub\tiebreak_wc\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{459AD3EE-165C-4EC2-B910-3142B2A017C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{523FAC44-5378-4433-9707-202A02268821}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="96B11" sheetId="1" r:id="rId1"/>
@@ -34,8 +34,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -166,7 +166,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,30 +183,18 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -253,34 +241,31 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="6"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="6"/>
   </cellXfs>
-  <cellStyles count="8">
-    <cellStyle name="20% - Accent6" xfId="5" builtinId="50"/>
-    <cellStyle name="40% - Accent1" xfId="2" builtinId="31"/>
-    <cellStyle name="40% - Accent4" xfId="3" builtinId="43"/>
-    <cellStyle name="40% - Accent6" xfId="4" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="7" builtinId="52"/>
-    <cellStyle name="Bad" xfId="6" builtinId="27"/>
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
+  <cellStyles count="7">
+    <cellStyle name="20% - Accent6" xfId="4" builtinId="50"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="40% - Accent4" xfId="2" builtinId="43"/>
+    <cellStyle name="40% - Accent6" xfId="3" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="6" builtinId="52"/>
+    <cellStyle name="Bad" xfId="5" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -562,26 +547,26 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -604,7 +589,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>8</v>
       </c>
@@ -648,7 +633,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>7</v>
       </c>
@@ -677,7 +662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -693,20 +678,20 @@
       <c r="H8" t="s">
         <v>11</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="4">
         <f>SUMPRODUCT(($B$6:$B$8=I5)*$D$6:$D$8 + ($C$6:$C$8=I5)*$E$6:$E$8)</f>
         <v>1</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="4">
         <f>SUMPRODUCT(($B$6:$B$8=J5)*$D$6:$D$8 + ($C$6:$C$8=J5)*$E$6:$E$8)</f>
         <v>1</v>
       </c>
-      <c r="K8" s="4">
+      <c r="K8" s="6">
         <f>SUMPRODUCT(($B$6:$B$8=K5)*$D$6:$D$8 + ($C$6:$C$8=K5)*$E$6:$E$8)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="H9" t="s">
         <v>12</v>
       </c>
@@ -723,7 +708,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E12" t="s">
         <v>13</v>
       </c>
@@ -731,7 +716,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E13" t="s">
         <v>14</v>
       </c>
@@ -742,7 +727,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E14" t="s">
         <v>19</v>
       </c>
@@ -763,26 +748,26 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -805,7 +790,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>16</v>
       </c>
@@ -849,7 +834,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>17</v>
       </c>
@@ -878,7 +863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>16</v>
       </c>
@@ -898,16 +883,16 @@
         <f>SUMPRODUCT(($B$6:$B$8=I5)*$D$6:$D$8 + ($C$6:$C$8=I5)*$E$6:$E$8)</f>
         <v>2</v>
       </c>
-      <c r="J8" s="7">
+      <c r="J8" s="6">
         <f>SUMPRODUCT(($B$6:$B$8=J5)*$D$6:$D$8 + ($C$6:$C$8=J5)*$E$6:$E$8)</f>
         <v>3</v>
       </c>
-      <c r="K8" s="5">
+      <c r="K8" s="4">
         <f>SUMPRODUCT(($B$6:$B$8=K5)*$D$6:$D$8 + ($C$6:$C$8=K5)*$E$6:$E$8)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="H9" t="s">
         <v>12</v>
       </c>
@@ -924,7 +909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E12" t="s">
         <v>13</v>
       </c>
@@ -935,7 +920,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E13" t="s">
         <v>14</v>
       </c>
@@ -946,7 +931,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E14" t="s">
         <v>19</v>
       </c>
@@ -970,23 +955,23 @@
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -1009,7 +994,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>21</v>
       </c>
@@ -1053,7 +1038,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>23</v>
       </c>
@@ -1069,11 +1054,11 @@
       <c r="H7" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="6">
         <f>I8-I9</f>
         <v>2</v>
       </c>
-      <c r="J7" s="5">
+      <c r="J7" s="4">
         <f>J8-J9</f>
         <v>-2</v>
       </c>
@@ -1082,7 +1067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>23</v>
       </c>
@@ -1111,7 +1096,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="H9" t="s">
         <v>12</v>
       </c>
@@ -1128,7 +1113,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E12" t="s">
         <v>13</v>
       </c>
@@ -1139,7 +1124,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E13" t="s">
         <v>14</v>
       </c>
@@ -1150,7 +1135,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E14" t="s">
         <v>19</v>
       </c>
@@ -1171,26 +1156,26 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -1213,7 +1198,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>27</v>
       </c>
@@ -1257,7 +1242,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>16</v>
       </c>
@@ -1286,7 +1271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>28</v>
       </c>
@@ -1302,20 +1287,20 @@
       <c r="H8" t="s">
         <v>11</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="6">
         <f>SUMPRODUCT(($B$6:$B$8=I5)*$D$6:$D$8 + ($C$6:$C$8=I5)*$E$6:$E$8)</f>
         <v>3</v>
       </c>
-      <c r="J8" s="6">
+      <c r="J8" s="5">
         <f>SUMPRODUCT(($B$6:$B$8=J5)*$D$6:$D$8 + ($C$6:$C$8=J5)*$E$6:$E$8)</f>
         <v>1</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="6">
         <f>SUMPRODUCT(($B$6:$B$8=K5)*$D$6:$D$8 + ($C$6:$C$8=K5)*$E$6:$E$8)</f>
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="H9" t="s">
         <v>12</v>
       </c>
@@ -1332,7 +1317,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E12" t="s">
         <v>13</v>
       </c>
@@ -1343,7 +1328,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E13" t="s">
         <v>14</v>
       </c>
@@ -1351,7 +1336,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E14" t="s">
         <v>19</v>
       </c>
@@ -1372,26 +1357,26 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -1414,7 +1399,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>8</v>
       </c>
@@ -1458,7 +1443,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>17</v>
       </c>
@@ -1487,7 +1472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>29</v>
       </c>
@@ -1503,20 +1488,20 @@
       <c r="H8" t="s">
         <v>11</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="4">
         <f>SUMPRODUCT(($B$6:$B$8=I5)*$D$6:$D$8 + ($C$6:$C$8=I5)*$E$6:$E$8)</f>
         <v>1</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="4">
         <f>SUMPRODUCT(($B$6:$B$8=J5)*$D$6:$D$8 + ($C$6:$C$8=J5)*$E$6:$E$8)</f>
         <v>1</v>
       </c>
-      <c r="K8" s="5">
+      <c r="K8" s="6">
         <f>SUMPRODUCT(($B$6:$B$8=K5)*$D$6:$D$8 + ($C$6:$C$8=K5)*$E$6:$E$8)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="H9" t="s">
         <v>12</v>
       </c>
@@ -1533,7 +1518,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E12" t="s">
         <v>13</v>
       </c>
@@ -1544,7 +1529,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E13" t="s">
         <v>14</v>
       </c>
@@ -1555,7 +1540,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E14" t="s">
         <v>19</v>
       </c>
@@ -1572,27 +1557,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4CE4F59-4837-48A6-9080-73D14AC26ADB}">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -1615,7 +1600,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>16</v>
       </c>
@@ -1659,7 +1644,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>34</v>
       </c>
@@ -1688,7 +1673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>21</v>
       </c>
@@ -1704,20 +1689,20 @@
       <c r="H8" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="4">
         <f>SUMPRODUCT(($B$6:$B$8=I5)*$D$6:$D$8 + ($C$6:$C$8=I5)*$E$6:$E$8)</f>
         <v>1</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="6">
         <f>SUMPRODUCT(($B$6:$B$8=J5)*$D$6:$D$8 + ($C$6:$C$8=J5)*$E$6:$E$8)</f>
         <v>2</v>
       </c>
-      <c r="K8" s="3">
+      <c r="K8" s="6">
         <f>SUMPRODUCT(($B$6:$B$8=K5)*$D$6:$D$8 + ($C$6:$C$8=K5)*$E$6:$E$8)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="H9" t="s">
         <v>12</v>
       </c>
@@ -1734,7 +1719,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E12" t="s">
         <v>13</v>
       </c>
@@ -1745,7 +1730,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E13" t="s">
         <v>14</v>
       </c>
@@ -1756,7 +1741,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E14" t="s">
         <v>19</v>
       </c>
@@ -1777,23 +1762,23 @@
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -1816,7 +1801,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>16</v>
       </c>
@@ -1860,7 +1845,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>34</v>
       </c>
@@ -1880,16 +1865,16 @@
         <f>I8-I9</f>
         <v>0</v>
       </c>
-      <c r="J7" s="7">
+      <c r="J7" s="6">
         <f>J8-J9</f>
         <v>1</v>
       </c>
-      <c r="K7" s="5">
+      <c r="K7" s="4">
         <f>K8-K9</f>
         <v>-1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>21</v>
       </c>
@@ -1918,7 +1903,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="H9" t="s">
         <v>12</v>
       </c>
@@ -1935,7 +1920,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E12" t="s">
         <v>13</v>
       </c>
@@ -1946,7 +1931,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E13" t="s">
         <v>14</v>
       </c>
@@ -1957,7 +1942,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E14" t="s">
         <v>19</v>
       </c>
@@ -1974,27 +1959,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F79C16B0-54AD-4EAA-9718-34CF760F8A43}">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -2017,7 +2002,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>16</v>
       </c>
@@ -2061,7 +2046,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>34</v>
       </c>
@@ -2081,16 +2066,16 @@
         <f>I8-I9</f>
         <v>0</v>
       </c>
-      <c r="J7" s="7">
+      <c r="J7" s="6">
         <f>J8-J9</f>
         <v>1</v>
       </c>
-      <c r="K7" s="5">
+      <c r="K7" s="4">
         <f>K8-K9</f>
         <v>-1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>21</v>
       </c>
@@ -2119,7 +2104,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="H9" t="s">
         <v>12</v>
       </c>
@@ -2136,7 +2121,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E12" t="s">
         <v>13</v>
       </c>
@@ -2147,7 +2132,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E13" t="s">
         <v>14</v>
       </c>
@@ -2158,7 +2143,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E14" t="s">
         <v>19</v>
       </c>

</xml_diff>